<commit_message>
add conversion to arctos
</commit_message>
<xml_diff>
--- a/input/Lewis_reviewed.xlsx
+++ b/input/Lewis_reviewed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48EB4410-4165-4FC9-BD62-A42197064C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C14C180A-C9EC-495D-A950-9D0E4F3C7748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>Lewis</t>
   </si>
   <si>
-    <t>Lewis2783</t>
+    <t>Lewis2775</t>
   </si>
   <si>
     <t>Amalaraeus fossoris Sutemin, 1969</t>
@@ -190,7 +190,7 @@
     <t>Amalaraeus sugitanii Sutemin, 1969 (nomina ex phantasia)</t>
   </si>
   <si>
-    <t>Lewis2784</t>
+    <t>Lewis2776</t>
   </si>
   <si>
     <t>Amalaraeus sugitanii Sutemin, 1969</t>
@@ -208,7 +208,7 @@
     <t>Ceratophyllus sterni Curt., [1829] (cited in Dale, 1878, but no associated valid species)</t>
   </si>
   <si>
-    <t>Lewis2785</t>
+    <t>Lewis2777</t>
   </si>
   <si>
     <t>Ceratophyllus sterni Curt., [1829]</t>
@@ -232,7 +232,7 @@
     <t>Ctenophthalmus flavus Suteminn, 1969 (nomina ex phantasia)</t>
   </si>
   <si>
-    <t>Lewis2786</t>
+    <t>Lewis2778</t>
   </si>
   <si>
     <t>Ctenophthalmus flavus Suteminn, 1969</t>
@@ -250,7 +250,7 @@
     <t>Ctenophthalmus nepalensis Sutemin, 1969 (nomina ex phantasia)</t>
   </si>
   <si>
-    <t>Lewis2787</t>
+    <t>Lewis2779</t>
   </si>
   <si>
     <t>Ctenophthalmus nepalensis Sutemin, 1969</t>
@@ -268,7 +268,7 @@
     <t>Pulex gigas Kirby, 1837 (likely a species of Hystrichopsylla)</t>
   </si>
   <si>
-    <t>Lewis2788</t>
+    <t>Lewis2780</t>
   </si>
   <si>
     <t>Pulex gigas Kirby, 1837</t>
@@ -289,7 +289,7 @@
     <t>Pulex imperator Westwood, 1858 (non-flea)</t>
   </si>
   <si>
-    <t>Lewis2789</t>
+    <t>Lewis2781</t>
   </si>
   <si>
     <t>Pulex imperator Westwood, 1858</t>
@@ -310,7 +310,7 @@
     <t>Pulex terrestris ferox Alpinus, 1874 (nomina ex phantasia)</t>
   </si>
   <si>
-    <t>Lewis2790</t>
+    <t>Lewis2782</t>
   </si>
   <si>
     <t>Pulex terrestris ferox Alpinus, 1874</t>
@@ -349,7 +349,7 @@
     <t>Amphipsylla kuznetzovi transcaucasica Goncharov, 1973 (junior homonym)</t>
   </si>
   <si>
-    <t>Lewis2805</t>
+    <t>Lewis2797</t>
   </si>
   <si>
     <t>Lewis156</t>
@@ -388,7 +388,7 @@
     <t>Pulex hirundinis Köhler, 1832 (junior homonym); Ceratophyllus hirundinis Chao, 1947 (junior homonym); Ceratophyllus hirundinis oiticus Peus, 1954; Ceratophyllus phaulius Rothschild, 1909; Ceratophyllus pinnatus Wagner, 1898; Ceratophyllus troglodytes Dampf, 1908</t>
   </si>
   <si>
-    <t>Lewis2822</t>
+    <t>Lewis2814</t>
   </si>
   <si>
     <t>Lewis338</t>
@@ -418,7 +418,7 @@
     <t>Pulex canis Curtis, 1826 (junior homonym); Pulex canis Dugès, 1832 (junior homonym); Ctenocephalus novemdentatus Kolenati, 1859</t>
   </si>
   <si>
-    <t>Lewis2849</t>
+    <t>Lewis2841</t>
   </si>
   <si>
     <t>Lewis517</t>
@@ -454,7 +454,7 @@
     <t>Ectinorus onychius angularis Smit &amp; Rosicky, 1987 (elevated to specific status by Hastriter &amp; Sage 2011)</t>
   </si>
   <si>
-    <t>Lewis2865</t>
+    <t>Lewis2857</t>
   </si>
   <si>
     <t>Lewis947</t>
@@ -487,7 +487,7 @@
     <t>Ectinorus onychius deplexus Smit, 1987 (elevated to specific status by Hastriter &amp; Sage 2011)</t>
   </si>
   <si>
-    <t>Lewis2867</t>
+    <t>Lewis2859</t>
   </si>
   <si>
     <t>Lewis954</t>
@@ -511,7 +511,7 @@
     <t>Ectinorus onychius fueginus Jordan, 1942 (placed as synonym by Hastriter and Sage 2011)</t>
   </si>
   <si>
-    <t>Lewis2868</t>
+    <t>Lewis2860</t>
   </si>
   <si>
     <t>Lewis973</t>
@@ -547,7 +547,7 @@
     <t>Frontopsylla tuoli Yu &amp; Zhang, 1981 (misapplication of F. tuoliensis)</t>
   </si>
   <si>
-    <t>Lewis2880</t>
+    <t>Lewis2872</t>
   </si>
   <si>
     <t>Lewis1078</t>
@@ -580,7 +580,7 @@
     <t>Pulex talpae Bouche, 1835 (junior homonym of Pulex fasciatus Bosc, 1800); Pulex furoris Dale, 1878; Ceratophyllus canadensis Baker, 1904; Ceratophyllus californicus Baker, 1904; Ceratophyllus endymionis Rothschild, 1904; Ceratophyllus oculatus Baker, 1904; Nosopsyllus paganus Peus, 1949</t>
   </si>
   <si>
-    <t>Lewis2937</t>
+    <t>Lewis2929</t>
   </si>
   <si>
     <t>Lewis1702</t>
@@ -616,7 +616,7 @@
     <t>Opisodasys jellisoni I. Fox, 1941 [female Opisodasys vesperalis (Jordan, 1929)]</t>
   </si>
   <si>
-    <t>Lewis2950</t>
+    <t>Lewis2942</t>
   </si>
   <si>
     <t>Lewis1829</t>
@@ -649,7 +649,7 @@
     <t>Palaeopsylla makaluensis Brelih, 1975 (Female)</t>
   </si>
   <si>
-    <t>Lewis2962</t>
+    <t>Lewis2954</t>
   </si>
   <si>
     <t>Lewis1882</t>
@@ -682,7 +682,7 @@
     <t>Paradoxopsyllus cruvispinus (sic) Miyajima &amp; Koidzumi, 1909; Ceratophyllus subcaecatus Rothschild, 1912</t>
   </si>
   <si>
-    <t>Lewis2969</t>
+    <t>Lewis2961</t>
   </si>
   <si>
     <t>Lewis2001</t>
@@ -718,7 +718,7 @@
     <t>Polygenis platensis cisandinus (Jordan, 1939)</t>
   </si>
   <si>
-    <t>Lewis2985</t>
+    <t>Lewis2977</t>
   </si>
   <si>
     <t>Lewis2218</t>
@@ -748,7 +748,7 @@
     <t>Pygiopsylla congrua Jordan &amp; Rothschild, 1922 (female); Pygiopsylla spinata Holland, 1969</t>
   </si>
   <si>
-    <t>Lewis2994</t>
+    <t>Lewis2986</t>
   </si>
   <si>
     <t>Lewis2257</t>
@@ -781,7 +781,7 @@
     <t>Pygiopsylla congrua Jordan &amp; Rothschild, 1922 (male)</t>
   </si>
   <si>
-    <t>Lewis2995</t>
+    <t>Lewis2987</t>
   </si>
   <si>
     <t>Lewis2260</t>
@@ -808,7 +808,7 @@
     <t>Stenoponia tripectinata ssp. barcana, blanda, irakana, medialis, separata spinellosa Jordan, 1958 (see Beaucournu, 2013)</t>
   </si>
   <si>
-    <t>Lewis3017</t>
+    <t>Lewis3009</t>
   </si>
   <si>
     <t>Lewis2452</t>
@@ -841,7 +841,7 @@
     <t>Thrassis howelli (Jordan, 1933); Thrassis acamantis Stark, 1970; Thrassis pristinus Stark, 1957; Thrassis utahensis Wagner, 1936</t>
   </si>
   <si>
-    <t>Lewis3023</t>
+    <t>Lewis3015</t>
   </si>
   <si>
     <t>Lewis2533</t>
@@ -868,7 +868,7 @@
     <t>Xenopsylla skrjabini Ioff, 1928 (only later 1930 did Ioff describe)</t>
   </si>
   <si>
-    <t>Lewis3042</t>
+    <t>Lewis3034</t>
   </si>
   <si>
     <t>Lewis2710</t>
@@ -898,7 +898,7 @@
     <t>Ceratophyllus mustelae Wagner, 1898 (junior homonym)</t>
   </si>
   <si>
-    <t>Lewis3052</t>
+    <t>Lewis3044</t>
   </si>
   <si>
     <t>Lewis84</t>
@@ -931,7 +931,7 @@
     <t>Typhlopsylla sibirica Wagner, 1901 (junior homonym); Ceratophyllus thoracicus Rothschild, 1911</t>
   </si>
   <si>
-    <t>Lewis3058</t>
+    <t>Lewis3050</t>
   </si>
   <si>
     <t>Lewis153</t>
@@ -961,7 +961,7 @@
     <t>Ceratophyllus chaoi Wang, 1957 (junior homonym)</t>
   </si>
   <si>
-    <t>Lewis3068</t>
+    <t>Lewis3060</t>
   </si>
   <si>
     <t>Lewis328</t>
@@ -991,7 +991,7 @@
     <t>Ctenophthalmus agyrtes slovacicus Rosicky, 1951 (partim); Ctenophthalmus orphilus tatricus Rosicky, 1951 (partim); Ctenophthalmus agyrtes obenbergeri Rosicky, 1957</t>
   </si>
   <si>
-    <t>Lewis3083</t>
+    <t>Lewis3075</t>
   </si>
   <si>
     <t>Lewis549</t>
@@ -1027,7 +1027,7 @@
     <t>Palaeopsylla makaluensis Brelih, 1975 (Male)</t>
   </si>
   <si>
-    <t>Lewis3144</t>
+    <t>Lewis3136</t>
   </si>
   <si>
     <t>Lewis1941</t>
@@ -1051,834 +1051,834 @@
     <t>Rhadinopsylla acuminata Ioff &amp; Tiflov, 1946 (suppressed by ICZN)</t>
   </si>
   <si>
+    <t>Lewis3147</t>
+  </si>
+  <si>
+    <t>Lewis2314</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla acuminata Ioff &amp; Tiflov, 1946</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla li transbaikalica Ioff &amp; Tiflov, 1947</t>
+  </si>
+  <si>
+    <t>acuminata</t>
+  </si>
+  <si>
+    <t>Ioff &amp; Tiflov, 1946</t>
+  </si>
+  <si>
+    <t>suppressed by ICZN</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla acuminata</t>
+  </si>
+  <si>
+    <t>Monopsyllus</t>
+  </si>
+  <si>
+    <t>thamba</t>
+  </si>
+  <si>
+    <t>Ceratophyllus bakeri Wagner, 1933; Monopsyllus enderleini Wagner, 1933 (?)</t>
+  </si>
+  <si>
+    <t>Lewis3169</t>
+  </si>
+  <si>
+    <t>Lewis43</t>
+  </si>
+  <si>
+    <t>Monopsyllus enderleini Wagner, 1933</t>
+  </si>
+  <si>
+    <t>Aetheca thamba (Jordan, 1929)</t>
+  </si>
+  <si>
+    <t>enderleini</t>
+  </si>
+  <si>
+    <t>Wagner, 1933</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Monopsyllus enderleini</t>
+  </si>
+  <si>
+    <t>Lewis3178</t>
+  </si>
+  <si>
+    <t>Ceratophyllus hirundinis Chao, 1947</t>
+  </si>
+  <si>
+    <t>Chao, 1947</t>
+  </si>
+  <si>
+    <t>Ceratophyllus hirundinis</t>
+  </si>
+  <si>
+    <t>Lewis3186</t>
+  </si>
+  <si>
+    <t>Pulex canis Dugès, 1832</t>
+  </si>
+  <si>
+    <t>Dugès, 1832</t>
+  </si>
+  <si>
+    <t>Ischnopsyllidae</t>
+  </si>
+  <si>
+    <t>Ischnopsyllinae</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus</t>
+  </si>
+  <si>
+    <t>intermedius</t>
+  </si>
+  <si>
+    <t>Ceratopsylla wagneri Kohaut, 1903; Ischnopsyllus schmitzi Oudemans, 1909 (female Ischnopsyllus intermedius)</t>
+  </si>
+  <si>
+    <t>Lewis3196</t>
+  </si>
+  <si>
+    <t>Lewis1215</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus schmitzi Oudemans, 1909</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus intermedius (Rothschild, 1898)</t>
+  </si>
+  <si>
+    <t>schmitzi</t>
+  </si>
+  <si>
+    <t>Oudemans, 1909</t>
+  </si>
+  <si>
+    <t>female Ischnopsyllus intermedius</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus schmitzi</t>
+  </si>
+  <si>
+    <t>needhami</t>
+  </si>
+  <si>
+    <t>Hsu</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus wassilii Scalon 1935; Ischnopsyllus vasilii Skalon (in Argyropulo, 1948)</t>
+  </si>
+  <si>
+    <t>Lewis3197</t>
+  </si>
+  <si>
+    <t>Lewis1220</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus vasilii Skalon</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus needhami Hsu, 1935</t>
+  </si>
+  <si>
+    <t>vasilii</t>
+  </si>
+  <si>
+    <t>Skalon</t>
+  </si>
+  <si>
+    <t>in Argyropulo, 1948</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus vasilii</t>
+  </si>
+  <si>
+    <t>Leptopsyllinae</t>
+  </si>
+  <si>
+    <t>segnis</t>
+  </si>
+  <si>
+    <t>(Schönherr)</t>
+  </si>
+  <si>
+    <t>Pulex musculi Dugès, 1832; Pulex musculi Bouché, 1835 (junior homonym of Pulex musculi Dugès, 1832); Ctenophthalmus quadridentatus Kolenati, 1859; Ctenophthalmus bisbidentatus Kolenati, 1859;Typhlopsylla mexicana Baker, 1896;</t>
+  </si>
+  <si>
+    <t>Lewis3199</t>
+  </si>
+  <si>
+    <t>Lewis1328</t>
+  </si>
+  <si>
+    <t>Pulex musculi Bouché, 1835</t>
+  </si>
+  <si>
+    <t>Leptopsylla segnis (Schönherr, 1811)</t>
+  </si>
+  <si>
+    <t>musculi</t>
+  </si>
+  <si>
+    <t>Bouché, 1835</t>
+  </si>
+  <si>
+    <t>junior homonym of Pulex musculi Dugès, 1832</t>
+  </si>
+  <si>
+    <t>Pulex musculi</t>
+  </si>
+  <si>
+    <t>Oropsylla</t>
+  </si>
+  <si>
+    <t>montana</t>
+  </si>
+  <si>
+    <t>(Baker)</t>
+  </si>
+  <si>
+    <t>Ceratophyllus acutus Baker, 1904; Oropsylla montana mandarina (Jordan &amp; Rothschild, 1911); Diamanus hopkinsi Vargas, 1955</t>
+  </si>
+  <si>
+    <t>Lewis3218</t>
+  </si>
+  <si>
+    <t>Lewis1859</t>
+  </si>
+  <si>
+    <t>Oropsylla montana mandarina</t>
+  </si>
+  <si>
+    <t>Oropsylla montana (Baker, 1895)</t>
+  </si>
+  <si>
+    <t>mandarina</t>
+  </si>
+  <si>
+    <t>isacantha</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla isacantha continentalis Smit, 1957; Rhadinopsylla pitymydis (Zavattari, 1914)</t>
+  </si>
+  <si>
+    <t>Lewis3232</t>
+  </si>
+  <si>
+    <t>Lewis2307</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla pitymydis</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla isacantha (Rothschild, 1907)</t>
+  </si>
+  <si>
+    <t>pitymydis</t>
+  </si>
+  <si>
+    <t>sectilis</t>
+  </si>
+  <si>
+    <t>Micropsylla peromyscus Dunn, 1923; Rhadinopsylla sectilis goodi (Hubbard, 1941)</t>
+  </si>
+  <si>
+    <t>Lewis3233</t>
+  </si>
+  <si>
+    <t>Lewis2332</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla sectilis goodi</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla sectilis Jordan &amp; Rothschild, 1923</t>
+  </si>
+  <si>
+    <t>goodi</t>
+  </si>
+  <si>
+    <t>pallidus</t>
+  </si>
+  <si>
+    <t>(Taschenberg)</t>
+  </si>
+  <si>
+    <t>Synosternus pallidus infestus Wagner, 1933; Pulex witherbyi Rothschild (in: Witherby, 1902)</t>
+  </si>
+  <si>
+    <t>Lewis3238</t>
+  </si>
+  <si>
+    <t>Lewis2511</t>
+  </si>
+  <si>
+    <t>Pulex witherbyi Rothschild</t>
+  </si>
+  <si>
+    <t>Synosternus pallidus (Taschenberg, 1880)</t>
+  </si>
+  <si>
+    <t>witherbyi</t>
+  </si>
+  <si>
+    <t>Rothschild</t>
+  </si>
+  <si>
+    <t>in: Witherby, 1902</t>
+  </si>
+  <si>
+    <t>Pulex witherbyi</t>
+  </si>
+  <si>
+    <t>Glauertidos</t>
+  </si>
+  <si>
+    <t>scintilla scintilla</t>
+  </si>
+  <si>
+    <t>(M. Rothschild)</t>
+  </si>
+  <si>
+    <t>Glauertia scintilla M. Rothschild, 1936; Glauertidos M. Rothschild, 1937 (nomen novum for Glauertia = Acanthopsylla Jordan &amp; Rothschild, 1922)</t>
+  </si>
+  <si>
+    <t>Lewis3250</t>
+  </si>
+  <si>
+    <t>Lewis19</t>
+  </si>
+  <si>
+    <t>Glauertidos M. Rothschild, 1937</t>
+  </si>
+  <si>
+    <t>Acanthopsylla scintilla scintilla (M. Rothschild, 1936)</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>M. Rothschild, 1937</t>
+  </si>
+  <si>
+    <t>nomen novum for Glauertia = Acanthopsylla Jordan &amp; Rothschild, 1922</t>
+  </si>
+  <si>
+    <t>Hystrichopsyllidae</t>
+  </si>
+  <si>
+    <t>Hystrichopsyllinae</t>
+  </si>
+  <si>
+    <t>Atyphoceras</t>
+  </si>
+  <si>
+    <t>multidentatus multidentatus</t>
+  </si>
+  <si>
+    <t>(C. Fox)</t>
+  </si>
+  <si>
+    <t>Atyphloceras artius Jordan 1933; Atyphoceras (sic) Atyphloceras felix Jordan, 1933</t>
+  </si>
+  <si>
+    <t>Lewis3257</t>
+  </si>
+  <si>
+    <t>Lewis213</t>
+  </si>
+  <si>
+    <t>Atyphoceras  Atyphloceras felix Jordan, 1933</t>
+  </si>
+  <si>
+    <t>Atyphloceras multidentatus multidentatus (C. Fox, 1909)</t>
+  </si>
+  <si>
+    <t>felix</t>
+  </si>
+  <si>
+    <t>Atyphloceras Jordan, 1933</t>
+  </si>
+  <si>
+    <t>Atyphoceras felix</t>
+  </si>
+  <si>
+    <t>Lewis3266</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus orphilus tatricus Rosicky, 1951</t>
+  </si>
+  <si>
+    <t>orphilus</t>
+  </si>
+  <si>
+    <t>tatricus</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus orphilus tatricus</t>
+  </si>
+  <si>
+    <t>mokrzeckyi</t>
+  </si>
+  <si>
+    <t>Ceratophyllus acutus Baker, 1904; Diamanus hopkinsi Vargas, 1955; Oropsylla montana mandarina (Jordan &amp; Rothschild, 1911); Ceratophyllus sucinus Jordan &amp; Rothschild, 1921</t>
+  </si>
+  <si>
+    <t>Lewis3314</t>
+  </si>
+  <si>
+    <t>Lewis1728</t>
+  </si>
+  <si>
+    <t>Nosopsyllus mokrzeckyi (Wagner, 1916)</t>
+  </si>
+  <si>
+    <t>octodecimdentata</t>
+  </si>
+  <si>
+    <t>(Kolenati)</t>
+  </si>
+  <si>
+    <t>Ceratophyllus uralensis Wagner, 1898; Ctenonotus octodecimdentata octodecimdentata Kolenati 1863; Opisodasys jellisoni I. Fox, 1941 (male Tarsopsylla octodecimdentata)</t>
+  </si>
+  <si>
+    <t>Lewis3320</t>
+  </si>
+  <si>
+    <t>Lewis2515</t>
+  </si>
+  <si>
+    <t>Opisodasys jellisoni I. Fox, 1941</t>
+  </si>
+  <si>
+    <t>Tarsopsylla octodecimdentata (Kolenati, 1863)</t>
+  </si>
+  <si>
+    <t>I. Fox, 1941</t>
+  </si>
+  <si>
+    <t>male Tarsopsylla octodecimdentata</t>
+  </si>
+  <si>
+    <t>Opisodasys jellisoni</t>
+  </si>
+  <si>
+    <t>simplex simplex</t>
+  </si>
+  <si>
+    <t>Ceratophyllus danubianus Rothschild, 1909; Citellophilus simplex domicae Rosicky, 1956; Ischnopsyllus schmitzi Oudemans, 1909 (male of Ischnopsyllus simplex simplex)</t>
+  </si>
+  <si>
+    <t>Lewis3330</t>
+  </si>
+  <si>
+    <t>Lewis444</t>
+  </si>
+  <si>
+    <t>Citellophilus simplex simplex (Wagner, 1902)</t>
+  </si>
+  <si>
+    <t>male of Ischnopsyllus simplex simplex</t>
+  </si>
+  <si>
+    <t>agyrtes agyrtes</t>
+  </si>
+  <si>
+    <t>(Heller)</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus agyrtoides Wahlgren, 1911; Ctenophthalmus agyrtes hanzaki Rosicky, 1951; Ctenophthalmus agyrtes slovacicus Rosicky, 1951 (partim); Ctenophthalmus orphilus tatricus Rosicky, 1951 (partim)</t>
+  </si>
+  <si>
+    <t>Lewis3332</t>
+  </si>
+  <si>
+    <t>Lewis538</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus agyrtes agyrtes (Heller, 1896)</t>
+  </si>
+  <si>
+    <t>Lewis3359</t>
+  </si>
+  <si>
+    <t>Doratopsyllinae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spalacopsylla </t>
+  </si>
+  <si>
+    <t>Ewing</t>
+  </si>
+  <si>
+    <t>Spalacopsylla Pinto, 1930 (junior synonym)</t>
+  </si>
+  <si>
+    <t>Lewis2735</t>
+  </si>
+  <si>
+    <t>Lewis41</t>
+  </si>
+  <si>
+    <t>Spalacopsylla Pinto, 1930</t>
+  </si>
+  <si>
+    <t>Adoratopsylla Ewing, 1925</t>
+  </si>
+  <si>
+    <t>Pinto, 1930</t>
+  </si>
+  <si>
+    <t>junior synonym</t>
+  </si>
+  <si>
+    <t>Vermipsyllidae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oncopsylla </t>
+  </si>
+  <si>
+    <t>Kohaut</t>
+  </si>
+  <si>
+    <t>Oncopsylla Wahlgren, 1903 (junior synonym); Achaetopsylla Argyropulo, 1948</t>
+  </si>
+  <si>
+    <t>Lewis2740</t>
+  </si>
+  <si>
+    <t>Lewis401</t>
+  </si>
+  <si>
+    <t>Oncopsylla Wahlgren, 1903</t>
+  </si>
+  <si>
+    <t>Chaetopsylla Kohaut, 1903</t>
+  </si>
+  <si>
+    <t>Wahlgren, 1903</t>
+  </si>
+  <si>
+    <t>Coptopsyllidae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paracoptopsylla </t>
+  </si>
+  <si>
+    <t>Paracoptopsylla Argyropulo, 1938 (subgenus of Coptopsylla); Macocoptopsylla Ioff, 1953; Neocoptopsylla Wagner, 1932</t>
+  </si>
+  <si>
+    <t>Lewis2741</t>
+  </si>
+  <si>
+    <t>Lewis489</t>
+  </si>
+  <si>
+    <t>Paracoptopsylla Argyropulo, 1938</t>
+  </si>
+  <si>
+    <t>Coptopsylla Jordan &amp; Rothschild, 1908</t>
+  </si>
+  <si>
+    <t>Argyropulo, 1938</t>
+  </si>
+  <si>
+    <t>subgenus of Coptopsylla</t>
+  </si>
+  <si>
+    <t>Kolenati</t>
+  </si>
+  <si>
+    <t>Spalacopsylla Kolenati, 1856 (junior synonym)</t>
+  </si>
+  <si>
+    <t>Lewis2744</t>
+  </si>
+  <si>
+    <t>Lewis828</t>
+  </si>
+  <si>
+    <t>Spalacopsylla Kolenati, 1856</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus Kolenati, 1856</t>
+  </si>
+  <si>
+    <t>Kolenati, 1856</t>
+  </si>
+  <si>
+    <t>Stivaliidae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migrastivalius </t>
+  </si>
+  <si>
+    <t>Traub</t>
+  </si>
+  <si>
+    <t>Migrastivalius Traub, 1980 (subgenus)</t>
+  </si>
+  <si>
+    <t>Lewis2750</t>
+  </si>
+  <si>
+    <t>Lewis1120</t>
+  </si>
+  <si>
+    <t>Migrastivalius Traub, 1980</t>
+  </si>
+  <si>
+    <t>Gryphopsylla Traub, 1957</t>
+  </si>
+  <si>
+    <t>Traub, 1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hystroceras </t>
+  </si>
+  <si>
+    <t>Taschenberg</t>
+  </si>
+  <si>
+    <t>Hystroceras Ioff &amp; Scalon, 1950 (unrecognized subgenus)</t>
+  </si>
+  <si>
+    <t>Lewis2752</t>
+  </si>
+  <si>
+    <t>Lewis1198</t>
+  </si>
+  <si>
+    <t>Hystroceras Ioff &amp; Scalon, 1950</t>
+  </si>
+  <si>
+    <t>Hystrichopsylla Taschenberg, 1880</t>
+  </si>
+  <si>
+    <t>Ioff &amp; Scalon, 1950</t>
+  </si>
+  <si>
+    <t>unrecognized subgenus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pleochaetoides </t>
+  </si>
+  <si>
+    <t>Pleochaetoides Augustson, 1944 (subgenus); Jellisonia Traub, 1944 (subgenus)</t>
+  </si>
+  <si>
+    <t>Lewis2754</t>
+  </si>
+  <si>
+    <t>Lewis1252</t>
+  </si>
+  <si>
+    <t>Pleochaetoides Augustson, 1944</t>
+  </si>
+  <si>
+    <t>Jellisonia Traub, 1944</t>
+  </si>
+  <si>
+    <t>Augustson, 1944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myodopsylloides </t>
+  </si>
+  <si>
+    <t>Myodopsylloides Augustson, 1941 (junior synonym)</t>
+  </si>
+  <si>
+    <t>Lewis2760</t>
+  </si>
+  <si>
+    <t>Lewis1574</t>
+  </si>
+  <si>
+    <t>Myodopsylloides Augustson, 1941</t>
+  </si>
+  <si>
+    <t>Myodopsylla Jordan &amp; Rothschild, 1911</t>
+  </si>
+  <si>
+    <t>Augustson, 1941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goniopsyllus </t>
+  </si>
+  <si>
+    <t>Goniopsyllus Baker, 1906 (preoccupied as genus of Crestacea, Jordan &amp; Rothschild, 1914 proposed Notiopsylla as nomen novum for Goniopsyllus)</t>
+  </si>
+  <si>
+    <t>Lewis2762</t>
+  </si>
+  <si>
+    <t>Lewis1763</t>
+  </si>
+  <si>
+    <t>Goniopsyllus Baker, 1906</t>
+  </si>
+  <si>
+    <t>Notiopsylla Jordan &amp; Rothschild, 1914</t>
+  </si>
+  <si>
+    <t>Baker, 1906</t>
+  </si>
+  <si>
+    <t>preoccupied as genus of Crestacea, Jordan &amp; Rothschild, 1914 proposed Notiopsylla as nomen novum for Goniopsyllus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectofrontia </t>
+  </si>
+  <si>
+    <t>Rectofrontia Wagner, 1930 (synonym of subgenus Actenophthalmus); Rangulpsylla Darskaya, 1949 (synonym of subgenus Actenophthalmus)</t>
+  </si>
+  <si>
+    <t>Lewis2766</t>
+  </si>
+  <si>
+    <t>Lewis2344</t>
+  </si>
+  <si>
+    <t>Rectofrontia Wagner, 1930</t>
+  </si>
+  <si>
+    <t>Rhadinopsylla Jordan &amp; Rothschild, 1912</t>
+  </si>
+  <si>
+    <t>Wagner, 1930</t>
+  </si>
+  <si>
+    <t>synonym of subgenus Actenophthalmus</t>
+  </si>
+  <si>
+    <t>Anomiopsyllinae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miochaeta </t>
+  </si>
+  <si>
+    <t>Miochaeta Good, 1942 (sunken subgenus)</t>
+  </si>
+  <si>
+    <t>Lewis2768</t>
+  </si>
+  <si>
+    <t>Lewis2427</t>
+  </si>
+  <si>
+    <t>Miochaeta Good, 1942</t>
+  </si>
+  <si>
+    <t>Stenistomera Rothschild, 1915</t>
+  </si>
+  <si>
+    <t>Good, 1942</t>
+  </si>
+  <si>
+    <t>sunken subgenus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomadopsylla </t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Nomadopsylla Stark, 1970 (junior synonym of Thrassis); Pandoropsylla Stark, 1970 (junior synonym of Thrassis); Thrassoides Stark, 1970 (junior synonym of Thrassis)</t>
+  </si>
+  <si>
+    <t>Lewis2771</t>
+  </si>
+  <si>
+    <t>Lewis2544</t>
+  </si>
+  <si>
+    <t>Nomadopsylla Stark, 1970</t>
+  </si>
+  <si>
+    <t>Thrassis Jordan, 1933</t>
+  </si>
+  <si>
+    <t>Stark, 1970</t>
+  </si>
+  <si>
+    <t>junior synonym of Thrassis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trichopsylla </t>
+  </si>
+  <si>
+    <t>Trichopsylla Kolenati, 1863; Trichopsylla Jordan &amp; Rothschild, 1920 (junior homonym of Trichopsylla Kolenati, 1863); Trichopsylla Ewing &amp; Fox, 1943 (junior homonym of Trichopsylla Kolenati, 1863)</t>
+  </si>
+  <si>
     <t>Lewis3155</t>
   </si>
   <si>
-    <t>Lewis2314</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla acuminata Ioff &amp; Tiflov, 1946</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla li transbaikalica Ioff &amp; Tiflov, 1947</t>
-  </si>
-  <si>
-    <t>acuminata</t>
-  </si>
-  <si>
-    <t>Ioff &amp; Tiflov, 1946</t>
-  </si>
-  <si>
-    <t>suppressed by ICZN</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla acuminata</t>
-  </si>
-  <si>
-    <t>Monopsyllus</t>
-  </si>
-  <si>
-    <t>thamba</t>
-  </si>
-  <si>
-    <t>Ceratophyllus bakeri Wagner, 1933; Monopsyllus enderleini Wagner, 1933 (?)</t>
-  </si>
-  <si>
-    <t>Lewis3177</t>
-  </si>
-  <si>
-    <t>Lewis43</t>
-  </si>
-  <si>
-    <t>Monopsyllus enderleini Wagner, 1933</t>
-  </si>
-  <si>
-    <t>Aetheca thamba (Jordan, 1929)</t>
-  </si>
-  <si>
-    <t>enderleini</t>
-  </si>
-  <si>
-    <t>Wagner, 1933</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Monopsyllus enderleini</t>
-  </si>
-  <si>
-    <t>Lewis3186</t>
-  </si>
-  <si>
-    <t>Ceratophyllus hirundinis Chao, 1947</t>
-  </si>
-  <si>
-    <t>Chao, 1947</t>
-  </si>
-  <si>
-    <t>Ceratophyllus hirundinis</t>
-  </si>
-  <si>
-    <t>Lewis3194</t>
-  </si>
-  <si>
-    <t>Pulex canis Dugès, 1832</t>
-  </si>
-  <si>
-    <t>Dugès, 1832</t>
-  </si>
-  <si>
-    <t>Ischnopsyllidae</t>
-  </si>
-  <si>
-    <t>Ischnopsyllinae</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus</t>
-  </si>
-  <si>
-    <t>intermedius</t>
-  </si>
-  <si>
-    <t>Ceratopsylla wagneri Kohaut, 1903; Ischnopsyllus schmitzi Oudemans, 1909 (female Ischnopsyllus intermedius)</t>
-  </si>
-  <si>
-    <t>Lewis3204</t>
-  </si>
-  <si>
-    <t>Lewis1215</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus schmitzi Oudemans, 1909</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus intermedius (Rothschild, 1898)</t>
-  </si>
-  <si>
-    <t>schmitzi</t>
-  </si>
-  <si>
-    <t>Oudemans, 1909</t>
-  </si>
-  <si>
-    <t>female Ischnopsyllus intermedius</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus schmitzi</t>
-  </si>
-  <si>
-    <t>needhami</t>
-  </si>
-  <si>
-    <t>Hsu</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus wassilii Scalon 1935; Ischnopsyllus vasilii Skalon (in Argyropulo, 1948)</t>
-  </si>
-  <si>
-    <t>Lewis3205</t>
-  </si>
-  <si>
-    <t>Lewis1220</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus vasilii Skalon</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus needhami Hsu, 1935</t>
-  </si>
-  <si>
-    <t>vasilii</t>
-  </si>
-  <si>
-    <t>Skalon</t>
-  </si>
-  <si>
-    <t>in Argyropulo, 1948</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus vasilii</t>
-  </si>
-  <si>
-    <t>Leptopsyllinae</t>
-  </si>
-  <si>
-    <t>segnis</t>
-  </si>
-  <si>
-    <t>(Schönherr)</t>
-  </si>
-  <si>
-    <t>Pulex musculi Dugès, 1832; Pulex musculi Bouché, 1835 (junior homonym of Pulex musculi Dugès, 1832); Ctenophthalmus quadridentatus Kolenati, 1859; Ctenophthalmus bisbidentatus Kolenati, 1859;Typhlopsylla mexicana Baker, 1896;</t>
-  </si>
-  <si>
-    <t>Lewis3207</t>
-  </si>
-  <si>
-    <t>Lewis1328</t>
-  </si>
-  <si>
-    <t>Pulex musculi Bouché, 1835</t>
-  </si>
-  <si>
-    <t>Leptopsylla segnis (Schönherr, 1811)</t>
-  </si>
-  <si>
-    <t>musculi</t>
-  </si>
-  <si>
-    <t>Bouché, 1835</t>
-  </si>
-  <si>
-    <t>junior homonym of Pulex musculi Dugès, 1832</t>
-  </si>
-  <si>
-    <t>Pulex musculi</t>
-  </si>
-  <si>
-    <t>Oropsylla</t>
-  </si>
-  <si>
-    <t>montana</t>
-  </si>
-  <si>
-    <t>(Baker)</t>
-  </si>
-  <si>
-    <t>Ceratophyllus acutus Baker, 1904; Oropsylla montana mandarina (Jordan &amp; Rothschild, 1911); Diamanus hopkinsi Vargas, 1955</t>
-  </si>
-  <si>
-    <t>Lewis3226</t>
-  </si>
-  <si>
-    <t>Lewis1859</t>
-  </si>
-  <si>
-    <t>Oropsylla montana mandarina</t>
-  </si>
-  <si>
-    <t>Oropsylla montana (Baker, 1895)</t>
-  </si>
-  <si>
-    <t>mandarina</t>
-  </si>
-  <si>
-    <t>isacantha</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla isacantha continentalis Smit, 1957; Rhadinopsylla pitymydis (Zavattari, 1914)</t>
-  </si>
-  <si>
-    <t>Lewis3240</t>
-  </si>
-  <si>
-    <t>Lewis2307</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla pitymydis</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla isacantha (Rothschild, 1907)</t>
-  </si>
-  <si>
-    <t>pitymydis</t>
-  </si>
-  <si>
-    <t>sectilis</t>
-  </si>
-  <si>
-    <t>Micropsylla peromyscus Dunn, 1923; Rhadinopsylla sectilis goodi (Hubbard, 1941)</t>
-  </si>
-  <si>
-    <t>Lewis3241</t>
-  </si>
-  <si>
-    <t>Lewis2332</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla sectilis goodi</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla sectilis Jordan &amp; Rothschild, 1923</t>
-  </si>
-  <si>
-    <t>goodi</t>
-  </si>
-  <si>
-    <t>pallidus</t>
-  </si>
-  <si>
-    <t>(Taschenberg)</t>
-  </si>
-  <si>
-    <t>Synosternus pallidus infestus Wagner, 1933; Pulex witherbyi Rothschild (in: Witherby, 1902)</t>
-  </si>
-  <si>
-    <t>Lewis3246</t>
-  </si>
-  <si>
-    <t>Lewis2511</t>
-  </si>
-  <si>
-    <t>Pulex witherbyi Rothschild</t>
-  </si>
-  <si>
-    <t>Synosternus pallidus (Taschenberg, 1880)</t>
-  </si>
-  <si>
-    <t>witherbyi</t>
-  </si>
-  <si>
-    <t>Rothschild</t>
-  </si>
-  <si>
-    <t>in: Witherby, 1902</t>
-  </si>
-  <si>
-    <t>Pulex witherbyi</t>
-  </si>
-  <si>
-    <t>Glauertidos</t>
-  </si>
-  <si>
-    <t>scintilla scintilla</t>
-  </si>
-  <si>
-    <t>(M. Rothschild)</t>
-  </si>
-  <si>
-    <t>Glauertia scintilla M. Rothschild, 1936; Glauertidos M. Rothschild, 1937 (nomen novum for Glauertia = Acanthopsylla Jordan &amp; Rothschild, 1922)</t>
-  </si>
-  <si>
-    <t>Lewis3258</t>
-  </si>
-  <si>
-    <t>Lewis19</t>
-  </si>
-  <si>
-    <t>Glauertidos M. Rothschild, 1937</t>
-  </si>
-  <si>
-    <t>Acanthopsylla scintilla scintilla (M. Rothschild, 1936)</t>
-  </si>
-  <si>
-    <t>review</t>
-  </si>
-  <si>
-    <t>M. Rothschild, 1937</t>
-  </si>
-  <si>
-    <t>nomen novum for Glauertia = Acanthopsylla Jordan &amp; Rothschild, 1922</t>
-  </si>
-  <si>
-    <t>Hystrichopsyllidae</t>
-  </si>
-  <si>
-    <t>Hystrichopsyllinae</t>
-  </si>
-  <si>
-    <t>Atyphoceras</t>
-  </si>
-  <si>
-    <t>multidentatus multidentatus</t>
-  </si>
-  <si>
-    <t>(C. Fox)</t>
-  </si>
-  <si>
-    <t>Atyphloceras artius Jordan 1933; Atyphoceras (sic) Atyphloceras felix Jordan, 1933</t>
-  </si>
-  <si>
-    <t>Lewis3265</t>
-  </si>
-  <si>
-    <t>Lewis213</t>
-  </si>
-  <si>
-    <t>Atyphoceras  Atyphloceras felix Jordan, 1933</t>
-  </si>
-  <si>
-    <t>Atyphloceras multidentatus multidentatus (C. Fox, 1909)</t>
-  </si>
-  <si>
-    <t>felix</t>
-  </si>
-  <si>
-    <t>Atyphloceras Jordan, 1933</t>
-  </si>
-  <si>
-    <t>Atyphoceras felix</t>
-  </si>
-  <si>
-    <t>Lewis3274</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus orphilus tatricus Rosicky, 1951</t>
-  </si>
-  <si>
-    <t>orphilus</t>
-  </si>
-  <si>
-    <t>tatricus</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus orphilus tatricus</t>
-  </si>
-  <si>
-    <t>mokrzeckyi</t>
-  </si>
-  <si>
-    <t>Ceratophyllus acutus Baker, 1904; Diamanus hopkinsi Vargas, 1955; Oropsylla montana mandarina (Jordan &amp; Rothschild, 1911); Ceratophyllus sucinus Jordan &amp; Rothschild, 1921</t>
-  </si>
-  <si>
-    <t>Lewis3322</t>
-  </si>
-  <si>
-    <t>Lewis1728</t>
-  </si>
-  <si>
-    <t>Nosopsyllus mokrzeckyi (Wagner, 1916)</t>
-  </si>
-  <si>
-    <t>octodecimdentata</t>
-  </si>
-  <si>
-    <t>(Kolenati)</t>
-  </si>
-  <si>
-    <t>Ceratophyllus uralensis Wagner, 1898; Ctenonotus octodecimdentata octodecimdentata Kolenati 1863; Opisodasys jellisoni I. Fox, 1941 (male Tarsopsylla octodecimdentata)</t>
-  </si>
-  <si>
-    <t>Lewis3328</t>
-  </si>
-  <si>
-    <t>Lewis2515</t>
-  </si>
-  <si>
-    <t>Opisodasys jellisoni I. Fox, 1941</t>
-  </si>
-  <si>
-    <t>Tarsopsylla octodecimdentata (Kolenati, 1863)</t>
-  </si>
-  <si>
-    <t>I. Fox, 1941</t>
-  </si>
-  <si>
-    <t>male Tarsopsylla octodecimdentata</t>
-  </si>
-  <si>
-    <t>Opisodasys jellisoni</t>
-  </si>
-  <si>
-    <t>simplex simplex</t>
-  </si>
-  <si>
-    <t>Ceratophyllus danubianus Rothschild, 1909; Citellophilus simplex domicae Rosicky, 1956; Ischnopsyllus schmitzi Oudemans, 1909 (male of Ischnopsyllus simplex simplex)</t>
-  </si>
-  <si>
-    <t>Lewis3338</t>
-  </si>
-  <si>
-    <t>Lewis444</t>
-  </si>
-  <si>
-    <t>Citellophilus simplex simplex (Wagner, 1902)</t>
-  </si>
-  <si>
-    <t>male of Ischnopsyllus simplex simplex</t>
-  </si>
-  <si>
-    <t>agyrtes agyrtes</t>
-  </si>
-  <si>
-    <t>(Heller)</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus agyrtoides Wahlgren, 1911; Ctenophthalmus agyrtes hanzaki Rosicky, 1951; Ctenophthalmus agyrtes slovacicus Rosicky, 1951 (partim); Ctenophthalmus orphilus tatricus Rosicky, 1951 (partim)</t>
-  </si>
-  <si>
-    <t>Lewis3340</t>
-  </si>
-  <si>
-    <t>Lewis538</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus agyrtes agyrtes (Heller, 1896)</t>
-  </si>
-  <si>
-    <t>Lewis3367</t>
-  </si>
-  <si>
-    <t>Doratopsyllinae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spalacopsylla </t>
-  </si>
-  <si>
-    <t>Ewing</t>
-  </si>
-  <si>
-    <t>Spalacopsylla Pinto, 1930 (junior synonym)</t>
-  </si>
-  <si>
-    <t>Lewis2743</t>
-  </si>
-  <si>
-    <t>Lewis41</t>
-  </si>
-  <si>
-    <t>Spalacopsylla Pinto, 1930</t>
-  </si>
-  <si>
-    <t>Adoratopsylla Ewing, 1925</t>
-  </si>
-  <si>
-    <t>Pinto, 1930</t>
-  </si>
-  <si>
-    <t>junior synonym</t>
-  </si>
-  <si>
-    <t>Vermipsyllidae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oncopsylla </t>
-  </si>
-  <si>
-    <t>Kohaut</t>
-  </si>
-  <si>
-    <t>Oncopsylla Wahlgren, 1903 (junior synonym); Achaetopsylla Argyropulo, 1948</t>
-  </si>
-  <si>
-    <t>Lewis2748</t>
-  </si>
-  <si>
-    <t>Lewis401</t>
-  </si>
-  <si>
-    <t>Oncopsylla Wahlgren, 1903</t>
-  </si>
-  <si>
-    <t>Chaetopsylla Kohaut, 1903</t>
-  </si>
-  <si>
-    <t>Wahlgren, 1903</t>
-  </si>
-  <si>
-    <t>Coptopsyllidae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paracoptopsylla </t>
-  </si>
-  <si>
-    <t>Paracoptopsylla Argyropulo, 1938 (subgenus of Coptopsylla); Macocoptopsylla Ioff, 1953; Neocoptopsylla Wagner, 1932</t>
-  </si>
-  <si>
-    <t>Lewis2749</t>
-  </si>
-  <si>
-    <t>Lewis489</t>
-  </si>
-  <si>
-    <t>Paracoptopsylla Argyropulo, 1938</t>
-  </si>
-  <si>
-    <t>Coptopsylla Jordan &amp; Rothschild, 1908</t>
-  </si>
-  <si>
-    <t>Argyropulo, 1938</t>
-  </si>
-  <si>
-    <t>subgenus of Coptopsylla</t>
-  </si>
-  <si>
-    <t>Kolenati</t>
-  </si>
-  <si>
-    <t>Spalacopsylla Kolenati, 1856 (junior synonym)</t>
-  </si>
-  <si>
-    <t>Lewis2752</t>
-  </si>
-  <si>
-    <t>Lewis828</t>
-  </si>
-  <si>
-    <t>Spalacopsylla Kolenati, 1856</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus Kolenati, 1856</t>
-  </si>
-  <si>
-    <t>Kolenati, 1856</t>
-  </si>
-  <si>
-    <t>Stivaliidae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migrastivalius </t>
-  </si>
-  <si>
-    <t>Traub</t>
-  </si>
-  <si>
-    <t>Migrastivalius Traub, 1980 (subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis2758</t>
-  </si>
-  <si>
-    <t>Lewis1120</t>
-  </si>
-  <si>
-    <t>Migrastivalius Traub, 1980</t>
-  </si>
-  <si>
-    <t>Gryphopsylla Traub, 1957</t>
-  </si>
-  <si>
-    <t>Traub, 1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hystroceras </t>
-  </si>
-  <si>
-    <t>Taschenberg</t>
-  </si>
-  <si>
-    <t>Hystroceras Ioff &amp; Scalon, 1950 (unrecognized subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis2760</t>
-  </si>
-  <si>
-    <t>Lewis1198</t>
-  </si>
-  <si>
-    <t>Hystroceras Ioff &amp; Scalon, 1950</t>
-  </si>
-  <si>
-    <t>Hystrichopsylla Taschenberg, 1880</t>
-  </si>
-  <si>
-    <t>Ioff &amp; Scalon, 1950</t>
-  </si>
-  <si>
-    <t>unrecognized subgenus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pleochaetoides </t>
-  </si>
-  <si>
-    <t>Pleochaetoides Augustson, 1944 (subgenus); Jellisonia Traub, 1944 (subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis2762</t>
-  </si>
-  <si>
-    <t>Lewis1252</t>
-  </si>
-  <si>
-    <t>Pleochaetoides Augustson, 1944</t>
-  </si>
-  <si>
-    <t>Jellisonia Traub, 1944</t>
-  </si>
-  <si>
-    <t>Augustson, 1944</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myodopsylloides </t>
-  </si>
-  <si>
-    <t>Myodopsylloides Augustson, 1941 (junior synonym)</t>
-  </si>
-  <si>
-    <t>Lewis2768</t>
-  </si>
-  <si>
-    <t>Lewis1574</t>
-  </si>
-  <si>
-    <t>Myodopsylloides Augustson, 1941</t>
-  </si>
-  <si>
-    <t>Myodopsylla Jordan &amp; Rothschild, 1911</t>
-  </si>
-  <si>
-    <t>Augustson, 1941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goniopsyllus </t>
-  </si>
-  <si>
-    <t>Goniopsyllus Baker, 1906 (preoccupied as genus of Crestacea, Jordan &amp; Rothschild, 1914 proposed Notiopsylla as nomen novum for Goniopsyllus)</t>
-  </si>
-  <si>
-    <t>Lewis2770</t>
-  </si>
-  <si>
-    <t>Lewis1763</t>
-  </si>
-  <si>
-    <t>Goniopsyllus Baker, 1906</t>
-  </si>
-  <si>
-    <t>Notiopsylla Jordan &amp; Rothschild, 1914</t>
-  </si>
-  <si>
-    <t>Baker, 1906</t>
-  </si>
-  <si>
-    <t>preoccupied as genus of Crestacea, Jordan &amp; Rothschild, 1914 proposed Notiopsylla as nomen novum for Goniopsyllus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rectofrontia </t>
-  </si>
-  <si>
-    <t>Rectofrontia Wagner, 1930 (synonym of subgenus Actenophthalmus); Rangulpsylla Darskaya, 1949 (synonym of subgenus Actenophthalmus)</t>
-  </si>
-  <si>
-    <t>Lewis2774</t>
-  </si>
-  <si>
-    <t>Lewis2344</t>
-  </si>
-  <si>
-    <t>Rectofrontia Wagner, 1930</t>
-  </si>
-  <si>
-    <t>Rhadinopsylla Jordan &amp; Rothschild, 1912</t>
-  </si>
-  <si>
-    <t>Wagner, 1930</t>
-  </si>
-  <si>
-    <t>synonym of subgenus Actenophthalmus</t>
-  </si>
-  <si>
-    <t>Anomiopsyllinae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miochaeta </t>
-  </si>
-  <si>
-    <t>Miochaeta Good, 1942 (sunken subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis2776</t>
-  </si>
-  <si>
-    <t>Lewis2427</t>
-  </si>
-  <si>
-    <t>Miochaeta Good, 1942</t>
-  </si>
-  <si>
-    <t>Stenistomera Rothschild, 1915</t>
-  </si>
-  <si>
-    <t>Good, 1942</t>
-  </si>
-  <si>
-    <t>sunken subgenus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nomadopsylla </t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Nomadopsylla Stark, 1970 (junior synonym of Thrassis); Pandoropsylla Stark, 1970 (junior synonym of Thrassis); Thrassoides Stark, 1970 (junior synonym of Thrassis)</t>
-  </si>
-  <si>
-    <t>Lewis2779</t>
-  </si>
-  <si>
-    <t>Lewis2544</t>
-  </si>
-  <si>
-    <t>Nomadopsylla Stark, 1970</t>
-  </si>
-  <si>
-    <t>Thrassis Jordan, 1933</t>
-  </si>
-  <si>
-    <t>Stark, 1970</t>
-  </si>
-  <si>
-    <t>junior synonym of Thrassis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trichopsylla </t>
-  </si>
-  <si>
-    <t>Trichopsylla Kolenati, 1863; Trichopsylla Jordan &amp; Rothschild, 1920 (junior homonym of Trichopsylla Kolenati, 1863); Trichopsylla Ewing &amp; Fox, 1943 (junior homonym of Trichopsylla Kolenati, 1863)</t>
+    <t>Lewis91</t>
+  </si>
+  <si>
+    <t>Trichopsylla Jordan &amp; Rothschild, 1920</t>
+  </si>
+  <si>
+    <t>Amalaraeus Ioff, 1936</t>
+  </si>
+  <si>
+    <t>Jordan &amp; Rothschild, 1920</t>
+  </si>
+  <si>
+    <t>junior homonym of Trichopsylla Kolenati, 1863</t>
+  </si>
+  <si>
+    <t>Westwood</t>
+  </si>
+  <si>
+    <t>Ceratopsylla Wagner, 1988??; Spalacopsylla Oudemans, 1906 (junior synonym)Nychopsyllus Eysell, 1913; Nycteridiphilis K. Dalla Torre, 1914; Hirtopsylla Argyropulo, 1948 (unrecognized subgenus)</t>
+  </si>
+  <si>
+    <t>Lewis3160</t>
+  </si>
+  <si>
+    <t>Lewis1234</t>
+  </si>
+  <si>
+    <t>Spalacopsylla Oudemans, 1906 Nychopsyllus Eysell, 1913</t>
+  </si>
+  <si>
+    <t>Ischnopsyllus Westwood, 1833</t>
+  </si>
+  <si>
+    <t>Oudemans, 1906 Nychopsyllus Eysell, 1913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jellisonia </t>
+  </si>
+  <si>
+    <t>Lewis3161</t>
+  </si>
+  <si>
+    <t>Traub, 1944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aneptescopsylla </t>
+  </si>
+  <si>
+    <t>Oudemans</t>
+  </si>
+  <si>
+    <t>Eptescopsylla I. Fox, 1940; Aneptescopsylla Ioff, 1953 (unrecognized subgenus); Dinycteridopsylla Ioff, 1953 (unrecognized subgenus); Hexanycteropsylla Ioff, 1953 (unrecognized subgenus)</t>
   </si>
   <si>
     <t>Lewis3163</t>
   </si>
   <si>
-    <t>Lewis91</t>
-  </si>
-  <si>
-    <t>Trichopsylla Jordan &amp; Rothschild, 1920</t>
-  </si>
-  <si>
-    <t>Amalaraeus Ioff, 1936</t>
-  </si>
-  <si>
-    <t>Jordan &amp; Rothschild, 1920</t>
-  </si>
-  <si>
-    <t>junior homonym of Trichopsylla Kolenati, 1863</t>
-  </si>
-  <si>
-    <t>Westwood</t>
-  </si>
-  <si>
-    <t>Ceratopsylla Wagner, 1988??; Spalacopsylla Oudemans, 1906 (junior synonym)Nychopsyllus Eysell, 1913; Nycteridiphilis K. Dalla Torre, 1914; Hirtopsylla Argyropulo, 1948 (unrecognized subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis3168</t>
-  </si>
-  <si>
-    <t>Lewis1234</t>
-  </si>
-  <si>
-    <t>Spalacopsylla Oudemans, 1906 Nychopsyllus Eysell, 1913</t>
-  </si>
-  <si>
-    <t>Ischnopsyllus Westwood, 1833</t>
-  </si>
-  <si>
-    <t>Oudemans, 1906 Nychopsyllus Eysell, 1913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jellisonia </t>
-  </si>
-  <si>
-    <t>Lewis3169</t>
-  </si>
-  <si>
-    <t>Traub, 1944</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aneptescopsylla </t>
-  </si>
-  <si>
-    <t>Oudemans</t>
-  </si>
-  <si>
-    <t>Eptescopsylla I. Fox, 1940; Aneptescopsylla Ioff, 1953 (unrecognized subgenus); Dinycteridopsylla Ioff, 1953 (unrecognized subgenus); Hexanycteropsylla Ioff, 1953 (unrecognized subgenus)</t>
-  </si>
-  <si>
-    <t>Lewis3171</t>
-  </si>
-  <si>
     <t>Lewis1785</t>
   </si>
   <si>
@@ -1894,7 +1894,7 @@
     <t xml:space="preserve">Rangulpsylla </t>
   </si>
   <si>
-    <t>Lewis3172</t>
+    <t>Lewis3164</t>
   </si>
   <si>
     <t>Rangulpsylla Darskaya, 1949</t>
@@ -1906,13 +1906,13 @@
     <t xml:space="preserve">Pandoropsylla </t>
   </si>
   <si>
-    <t>Lewis3173</t>
+    <t>Lewis3165</t>
   </si>
   <si>
     <t>Pandoropsylla Stark, 1970</t>
   </si>
   <si>
-    <t>Lewis3293</t>
+    <t>Lewis3285</t>
   </si>
   <si>
     <t>Trichopsylla Ewing &amp; Fox, 1943</t>
@@ -1924,7 +1924,7 @@
     <t xml:space="preserve">Dinycteridopsylla </t>
   </si>
   <si>
-    <t>Lewis3297</t>
+    <t>Lewis3289</t>
   </si>
   <si>
     <t>Dinycteridopsylla Ioff, 1953</t>
@@ -1933,7 +1933,7 @@
     <t xml:space="preserve">Thrassoides </t>
   </si>
   <si>
-    <t>Lewis3298</t>
+    <t>Lewis3290</t>
   </si>
   <si>
     <t>Thrassoides Stark, 1970</t>
@@ -1951,7 +1951,7 @@
     <t>Dermatophilus Guérin, 1840; Dermatophylus Lucas, 1839; Psammodes Gistel 1850 (1847?); Rhynchoprion Karsten, 1864; Sarcophaga Westwood, 1840</t>
   </si>
   <si>
-    <t>Lewis3299</t>
+    <t>Lewis3291</t>
   </si>
   <si>
     <t>Lewis2592</t>
@@ -1972,7 +1972,7 @@
     <t xml:space="preserve">Hirtopsylla </t>
   </si>
   <si>
-    <t>Lewis3349</t>
+    <t>Lewis3341</t>
   </si>
   <si>
     <t>Hirtopsylla Argyropulo, 1948</t>
@@ -1984,7 +1984,7 @@
     <t xml:space="preserve">Hexanycteropsylla </t>
   </si>
   <si>
-    <t>Lewis3350</t>
+    <t>Lewis3342</t>
   </si>
   <si>
     <t>Hexanycteropsylla Ioff, 1953</t>
@@ -3024,7 +3024,7 @@
         <v>43</v>
       </c>
       <c r="I2">
-        <v>3177</v>
+        <v>3169</v>
       </c>
       <c r="J2" t="s">
         <v>354</v>
@@ -3146,7 +3146,7 @@
         <v>43</v>
       </c>
       <c r="I3">
-        <v>3299</v>
+        <v>3291</v>
       </c>
       <c r="J3" t="s">
         <v>643</v>
@@ -3268,7 +3268,7 @@
         <v>43</v>
       </c>
       <c r="I4">
-        <v>2785</v>
+        <v>2777</v>
       </c>
       <c r="J4" t="s">
         <v>62</v>
@@ -3390,7 +3390,7 @@
         <v>43</v>
       </c>
       <c r="I5">
-        <v>2865</v>
+        <v>2857</v>
       </c>
       <c r="J5" t="s">
         <v>144</v>
@@ -3512,7 +3512,7 @@
         <v>43</v>
       </c>
       <c r="I6">
-        <v>2867</v>
+        <v>2859</v>
       </c>
       <c r="J6" t="s">
         <v>155</v>
@@ -3634,7 +3634,7 @@
         <v>43</v>
       </c>
       <c r="I7">
-        <v>2962</v>
+        <v>2954</v>
       </c>
       <c r="J7" t="s">
         <v>209</v>
@@ -3756,7 +3756,7 @@
         <v>43</v>
       </c>
       <c r="I8">
-        <v>2994</v>
+        <v>2986</v>
       </c>
       <c r="J8" t="s">
         <v>242</v>
@@ -3878,7 +3878,7 @@
         <v>43</v>
       </c>
       <c r="I9">
-        <v>3204</v>
+        <v>3196</v>
       </c>
       <c r="J9" t="s">
         <v>374</v>
@@ -4000,7 +4000,7 @@
         <v>43</v>
       </c>
       <c r="I10">
-        <v>2950</v>
+        <v>2942</v>
       </c>
       <c r="J10" t="s">
         <v>198</v>
@@ -4122,7 +4122,7 @@
         <v>43</v>
       </c>
       <c r="I11">
-        <v>3205</v>
+        <v>3197</v>
       </c>
       <c r="J11" t="s">
         <v>385</v>
@@ -4244,7 +4244,7 @@
         <v>43</v>
       </c>
       <c r="I12">
-        <v>3246</v>
+        <v>3238</v>
       </c>
       <c r="J12" t="s">
         <v>431</v>
@@ -4366,7 +4366,7 @@
         <v>43</v>
       </c>
       <c r="I13">
-        <v>2937</v>
+        <v>2929</v>
       </c>
       <c r="J13" t="s">
         <v>186</v>
@@ -4488,7 +4488,7 @@
         <v>43</v>
       </c>
       <c r="I14">
-        <v>3207</v>
+        <v>3199</v>
       </c>
       <c r="J14" t="s">
         <v>397</v>
@@ -4610,7 +4610,7 @@
         <v>43</v>
       </c>
       <c r="I15">
-        <v>3163</v>
+        <v>3155</v>
       </c>
       <c r="J15" t="s">
         <v>599</v>
@@ -4732,7 +4732,7 @@
         <v>43</v>
       </c>
       <c r="I16">
-        <v>3293</v>
+        <v>3285</v>
       </c>
       <c r="J16" t="s">
         <v>630</v>
@@ -4854,7 +4854,7 @@
         <v>43</v>
       </c>
       <c r="I17">
-        <v>2779</v>
+        <v>2771</v>
       </c>
       <c r="J17" t="s">
         <v>591</v>
@@ -4976,7 +4976,7 @@
         <v>43</v>
       </c>
       <c r="I18">
-        <v>3173</v>
+        <v>3165</v>
       </c>
       <c r="J18" t="s">
         <v>628</v>
@@ -5098,7 +5098,7 @@
         <v>43</v>
       </c>
       <c r="I19">
-        <v>3298</v>
+        <v>3290</v>
       </c>
       <c r="J19" t="s">
         <v>637</v>
@@ -5220,7 +5220,7 @@
         <v>43</v>
       </c>
       <c r="I20">
-        <v>2788</v>
+        <v>2780</v>
       </c>
       <c r="J20" t="s">
         <v>82</v>
@@ -5342,7 +5342,7 @@
         <v>43</v>
       </c>
       <c r="I21">
-        <v>2995</v>
+        <v>2987</v>
       </c>
       <c r="J21" t="s">
         <v>253</v>
@@ -5464,7 +5464,7 @@
         <v>43</v>
       </c>
       <c r="I22">
-        <v>3144</v>
+        <v>3136</v>
       </c>
       <c r="J22" t="s">
         <v>335</v>
@@ -5586,7 +5586,7 @@
         <v>43</v>
       </c>
       <c r="I23">
-        <v>3338</v>
+        <v>3330</v>
       </c>
       <c r="J23" t="s">
         <v>485</v>
@@ -5708,7 +5708,7 @@
         <v>43</v>
       </c>
       <c r="I24">
-        <v>3328</v>
+        <v>3320</v>
       </c>
       <c r="J24" t="s">
         <v>476</v>
@@ -5830,7 +5830,7 @@
         <v>43</v>
       </c>
       <c r="I25">
-        <v>2880</v>
+        <v>2872</v>
       </c>
       <c r="J25" t="s">
         <v>175</v>
@@ -5952,7 +5952,7 @@
         <v>43</v>
       </c>
       <c r="I26">
-        <v>3258</v>
+        <v>3250</v>
       </c>
       <c r="J26" t="s">
         <v>443</v>
@@ -6074,7 +6074,7 @@
         <v>43</v>
       </c>
       <c r="I27">
-        <v>2783</v>
+        <v>2775</v>
       </c>
       <c r="J27" t="s">
         <v>44</v>
@@ -6196,7 +6196,7 @@
         <v>43</v>
       </c>
       <c r="I28">
-        <v>2784</v>
+        <v>2776</v>
       </c>
       <c r="J28" t="s">
         <v>56</v>
@@ -6318,7 +6318,7 @@
         <v>43</v>
       </c>
       <c r="I29">
-        <v>2786</v>
+        <v>2778</v>
       </c>
       <c r="J29" t="s">
         <v>70</v>
@@ -6440,7 +6440,7 @@
         <v>43</v>
       </c>
       <c r="I30">
-        <v>2787</v>
+        <v>2779</v>
       </c>
       <c r="J30" t="s">
         <v>76</v>
@@ -6562,7 +6562,7 @@
         <v>43</v>
       </c>
       <c r="I31">
-        <v>2790</v>
+        <v>2782</v>
       </c>
       <c r="J31" t="s">
         <v>96</v>
@@ -6684,7 +6684,7 @@
         <v>43</v>
       </c>
       <c r="I32">
-        <v>2789</v>
+        <v>2781</v>
       </c>
       <c r="J32" t="s">
         <v>89</v>
@@ -6806,7 +6806,7 @@
         <v>43</v>
       </c>
       <c r="I33">
-        <v>3042</v>
+        <v>3034</v>
       </c>
       <c r="J33" t="s">
         <v>282</v>
@@ -6928,7 +6928,7 @@
         <v>43</v>
       </c>
       <c r="I34">
-        <v>3083</v>
+        <v>3075</v>
       </c>
       <c r="J34" t="s">
         <v>323</v>
@@ -7050,7 +7050,7 @@
         <v>43</v>
       </c>
       <c r="I35">
-        <v>3274</v>
+        <v>3266</v>
       </c>
       <c r="J35" t="s">
         <v>463</v>
@@ -7172,7 +7172,7 @@
         <v>43</v>
       </c>
       <c r="I36">
-        <v>3340</v>
+        <v>3332</v>
       </c>
       <c r="J36" t="s">
         <v>492</v>
@@ -7294,7 +7294,7 @@
         <v>43</v>
       </c>
       <c r="I37">
-        <v>3367</v>
+        <v>3359</v>
       </c>
       <c r="J37" t="s">
         <v>495</v>
@@ -7416,7 +7416,7 @@
         <v>43</v>
       </c>
       <c r="I38">
-        <v>2868</v>
+        <v>2860</v>
       </c>
       <c r="J38" t="s">
         <v>163</v>
@@ -7538,7 +7538,7 @@
         <v>43</v>
       </c>
       <c r="I39">
-        <v>2770</v>
+        <v>2762</v>
       </c>
       <c r="J39" t="s">
         <v>565</v>
@@ -7660,7 +7660,7 @@
         <v>43</v>
       </c>
       <c r="I40">
-        <v>3017</v>
+        <v>3009</v>
       </c>
       <c r="J40" t="s">
         <v>262</v>
@@ -7782,7 +7782,7 @@
         <v>43</v>
       </c>
       <c r="I41">
-        <v>2969</v>
+        <v>2961</v>
       </c>
       <c r="J41" t="s">
         <v>220</v>
@@ -7904,7 +7904,7 @@
         <v>43</v>
       </c>
       <c r="I42">
-        <v>3265</v>
+        <v>3257</v>
       </c>
       <c r="J42" t="s">
         <v>456</v>
@@ -8026,7 +8026,7 @@
         <v>43</v>
       </c>
       <c r="I43">
-        <v>2749</v>
+        <v>2741</v>
       </c>
       <c r="J43" t="s">
         <v>518</v>
@@ -8148,7 +8148,7 @@
         <v>43</v>
       </c>
       <c r="I44">
-        <v>2776</v>
+        <v>2768</v>
       </c>
       <c r="J44" t="s">
         <v>582</v>
@@ -8270,7 +8270,7 @@
         <v>43</v>
       </c>
       <c r="I45">
-        <v>3155</v>
+        <v>3147</v>
       </c>
       <c r="J45" t="s">
         <v>343</v>
@@ -8392,7 +8392,7 @@
         <v>43</v>
       </c>
       <c r="I46">
-        <v>2774</v>
+        <v>2766</v>
       </c>
       <c r="J46" t="s">
         <v>573</v>
@@ -8514,7 +8514,7 @@
         <v>43</v>
       </c>
       <c r="I47">
-        <v>3172</v>
+        <v>3164</v>
       </c>
       <c r="J47" t="s">
         <v>624</v>
@@ -8636,7 +8636,7 @@
         <v>43</v>
       </c>
       <c r="I48">
-        <v>2760</v>
+        <v>2752</v>
       </c>
       <c r="J48" t="s">
         <v>543</v>
@@ -8758,7 +8758,7 @@
         <v>43</v>
       </c>
       <c r="I49">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="J49" t="s">
         <v>618</v>
@@ -8880,7 +8880,7 @@
         <v>43</v>
       </c>
       <c r="I50">
-        <v>3297</v>
+        <v>3289</v>
       </c>
       <c r="J50" t="s">
         <v>634</v>
@@ -9002,7 +9002,7 @@
         <v>43</v>
       </c>
       <c r="I51">
-        <v>3349</v>
+        <v>3341</v>
       </c>
       <c r="J51" t="s">
         <v>650</v>
@@ -9124,7 +9124,7 @@
         <v>43</v>
       </c>
       <c r="I52">
-        <v>3350</v>
+        <v>3342</v>
       </c>
       <c r="J52" t="s">
         <v>654</v>
@@ -9246,7 +9246,7 @@
         <v>43</v>
       </c>
       <c r="I53">
-        <v>3241</v>
+        <v>3233</v>
       </c>
       <c r="J53" t="s">
         <v>423</v>
@@ -9368,7 +9368,7 @@
         <v>43</v>
       </c>
       <c r="I54">
-        <v>3226</v>
+        <v>3218</v>
       </c>
       <c r="J54" t="s">
         <v>409</v>
@@ -9490,7 +9490,7 @@
         <v>43</v>
       </c>
       <c r="I55">
-        <v>3322</v>
+        <v>3314</v>
       </c>
       <c r="J55" t="s">
         <v>470</v>
@@ -9612,7 +9612,7 @@
         <v>43</v>
       </c>
       <c r="I56">
-        <v>3023</v>
+        <v>3015</v>
       </c>
       <c r="J56" t="s">
         <v>273</v>
@@ -9734,7 +9734,7 @@
         <v>43</v>
       </c>
       <c r="I57">
-        <v>2985</v>
+        <v>2977</v>
       </c>
       <c r="J57" t="s">
         <v>232</v>
@@ -9856,7 +9856,7 @@
         <v>43</v>
       </c>
       <c r="I58">
-        <v>2805</v>
+        <v>2797</v>
       </c>
       <c r="J58" t="s">
         <v>109</v>
@@ -9978,7 +9978,7 @@
         <v>43</v>
       </c>
       <c r="I59">
-        <v>2822</v>
+        <v>2814</v>
       </c>
       <c r="J59" t="s">
         <v>122</v>
@@ -10100,7 +10100,7 @@
         <v>43</v>
       </c>
       <c r="I60">
-        <v>2849</v>
+        <v>2841</v>
       </c>
       <c r="J60" t="s">
         <v>132</v>
@@ -10222,7 +10222,7 @@
         <v>43</v>
       </c>
       <c r="I61">
-        <v>3052</v>
+        <v>3044</v>
       </c>
       <c r="J61" t="s">
         <v>292</v>
@@ -10344,7 +10344,7 @@
         <v>43</v>
       </c>
       <c r="I62">
-        <v>3058</v>
+        <v>3050</v>
       </c>
       <c r="J62" t="s">
         <v>303</v>
@@ -10466,7 +10466,7 @@
         <v>43</v>
       </c>
       <c r="I63">
-        <v>3068</v>
+        <v>3060</v>
       </c>
       <c r="J63" t="s">
         <v>313</v>
@@ -10588,7 +10588,7 @@
         <v>43</v>
       </c>
       <c r="I64">
-        <v>3186</v>
+        <v>3178</v>
       </c>
       <c r="J64" t="s">
         <v>362</v>
@@ -10710,7 +10710,7 @@
         <v>43</v>
       </c>
       <c r="I65">
-        <v>3194</v>
+        <v>3186</v>
       </c>
       <c r="J65" t="s">
         <v>366</v>
@@ -10832,7 +10832,7 @@
         <v>43</v>
       </c>
       <c r="I66">
-        <v>2743</v>
+        <v>2735</v>
       </c>
       <c r="J66" t="s">
         <v>500</v>
@@ -10954,7 +10954,7 @@
         <v>43</v>
       </c>
       <c r="I67">
-        <v>2748</v>
+        <v>2740</v>
       </c>
       <c r="J67" t="s">
         <v>510</v>
@@ -11076,7 +11076,7 @@
         <v>43</v>
       </c>
       <c r="I68">
-        <v>2752</v>
+        <v>2744</v>
       </c>
       <c r="J68" t="s">
         <v>526</v>
@@ -11198,7 +11198,7 @@
         <v>43</v>
       </c>
       <c r="I69">
-        <v>2768</v>
+        <v>2760</v>
       </c>
       <c r="J69" t="s">
         <v>558</v>
@@ -11320,7 +11320,7 @@
         <v>43</v>
       </c>
       <c r="I70">
-        <v>3168</v>
+        <v>3160</v>
       </c>
       <c r="J70" t="s">
         <v>607</v>
@@ -11442,7 +11442,7 @@
         <v>43</v>
       </c>
       <c r="I71">
-        <v>2758</v>
+        <v>2750</v>
       </c>
       <c r="J71" t="s">
         <v>535</v>
@@ -11564,7 +11564,7 @@
         <v>43</v>
       </c>
       <c r="I72">
-        <v>2762</v>
+        <v>2754</v>
       </c>
       <c r="J72" t="s">
         <v>551</v>
@@ -11686,7 +11686,7 @@
         <v>43</v>
       </c>
       <c r="I73">
-        <v>3169</v>
+        <v>3161</v>
       </c>
       <c r="J73" t="s">
         <v>613</v>
@@ -11808,7 +11808,7 @@
         <v>43</v>
       </c>
       <c r="I74">
-        <v>3240</v>
+        <v>3232</v>
       </c>
       <c r="J74" t="s">
         <v>416</v>
@@ -11905,7 +11905,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN75">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO75">
     <sortCondition ref="AM2:AM75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates for GBIF and taxotools
</commit_message>
<xml_diff>
--- a/input/Lewis_reviewed.xlsx
+++ b/input/Lewis_reviewed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09163CA4-535E-4E18-9C9E-16381580637C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31C7A931-B157-4804-B304-F5192564DA0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -208,6 +208,78 @@
     <t>Pulex terrestris ferox Alpinus, 1874</t>
   </si>
   <si>
+    <t>Sutemin, 1969</t>
+  </si>
+  <si>
+    <t>Curt., [1829]</t>
+  </si>
+  <si>
+    <t>Suteminn, 1969</t>
+  </si>
+  <si>
+    <t>Kirby, 1837</t>
+  </si>
+  <si>
+    <t>Westwood, 1858</t>
+  </si>
+  <si>
+    <t>Alpinus, 1874</t>
+  </si>
+  <si>
+    <t>Amalaraeus fossoris</t>
+  </si>
+  <si>
+    <t>Amalaraeus sugitanii</t>
+  </si>
+  <si>
+    <t>Ceratophyllus sterni</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus flavus</t>
+  </si>
+  <si>
+    <t>Ctenophthalmus nepalensis</t>
+  </si>
+  <si>
+    <t>Pulex gigas</t>
+  </si>
+  <si>
+    <t>Pulex imperator</t>
+  </si>
+  <si>
+    <t>Pulex terrestris ferox</t>
+  </si>
+  <si>
+    <t>subspecies</t>
+  </si>
+  <si>
+    <t>ferox</t>
+  </si>
+  <si>
+    <t>fossoris</t>
+  </si>
+  <si>
+    <t>sugitanii</t>
+  </si>
+  <si>
+    <t>sterni</t>
+  </si>
+  <si>
+    <t>flavus</t>
+  </si>
+  <si>
+    <t>nepalensis</t>
+  </si>
+  <si>
+    <t>gigas</t>
+  </si>
+  <si>
+    <t>imperator</t>
+  </si>
+  <si>
+    <t>terrestris</t>
+  </si>
+  <si>
     <t>Amalaraeus</t>
   </si>
   <si>
@@ -220,88 +292,16 @@
     <t>Pulex</t>
   </si>
   <si>
-    <t>fossoris</t>
-  </si>
-  <si>
-    <t>sugitanii</t>
-  </si>
-  <si>
-    <t>sterni</t>
-  </si>
-  <si>
-    <t>flavus</t>
-  </si>
-  <si>
-    <t>nepalensis</t>
-  </si>
-  <si>
-    <t>gigas</t>
-  </si>
-  <si>
-    <t>imperator</t>
+    <t>Ceratophyllidae</t>
+  </si>
+  <si>
+    <t>Hystrichopsyllidae</t>
+  </si>
+  <si>
+    <t>Pulicidae</t>
   </si>
   <si>
     <t>terrestris ferox</t>
-  </si>
-  <si>
-    <t>ferox</t>
-  </si>
-  <si>
-    <t>terrestris</t>
-  </si>
-  <si>
-    <t>Sutemin, 1969</t>
-  </si>
-  <si>
-    <t>Curt., [1829]</t>
-  </si>
-  <si>
-    <t>Suteminn, 1969</t>
-  </si>
-  <si>
-    <t>Kirby, 1837</t>
-  </si>
-  <si>
-    <t>Westwood, 1858</t>
-  </si>
-  <si>
-    <t>Alpinus, 1874</t>
-  </si>
-  <si>
-    <t>subspecies</t>
-  </si>
-  <si>
-    <t>Amalaraeus fossoris</t>
-  </si>
-  <si>
-    <t>Amalaraeus sugitanii</t>
-  </si>
-  <si>
-    <t>Ceratophyllus sterni</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus flavus</t>
-  </si>
-  <si>
-    <t>Ctenophthalmus nepalensis</t>
-  </si>
-  <si>
-    <t>Pulex gigas</t>
-  </si>
-  <si>
-    <t>Pulex imperator</t>
-  </si>
-  <si>
-    <t>Pulex terrestris ferox</t>
-  </si>
-  <si>
-    <t>Ceratophyllidae</t>
-  </si>
-  <si>
-    <t>Hystrichopsyllidae</t>
-  </si>
-  <si>
-    <t>Pulicidae</t>
   </si>
 </sst>
 </file>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1271,19 +1271,19 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -1355,7 +1355,7 @@
         <v>39</v>
       </c>
       <c r="AC2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="AD2" t="s">
         <v>39</v>
@@ -1367,7 +1367,7 @@
         <v>39</v>
       </c>
       <c r="AG2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="AH2" t="s">
         <v>39</v>
@@ -1385,24 +1385,24 @@
         <v>39</v>
       </c>
       <c r="AM2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
         <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -1474,7 +1474,7 @@
         <v>39</v>
       </c>
       <c r="AC3" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="AD3" t="s">
         <v>39</v>
@@ -1486,7 +1486,7 @@
         <v>39</v>
       </c>
       <c r="AG3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="AH3" t="s">
         <v>39</v>
@@ -1504,24 +1504,24 @@
         <v>39</v>
       </c>
       <c r="AM3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
         <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
@@ -1593,7 +1593,7 @@
         <v>39</v>
       </c>
       <c r="AC4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="AD4" t="s">
         <v>39</v>
@@ -1605,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="AG4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="AH4" t="s">
         <v>39</v>
@@ -1623,24 +1623,24 @@
         <v>39</v>
       </c>
       <c r="AM4" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -1712,7 +1712,7 @@
         <v>39</v>
       </c>
       <c r="AC5" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="AD5" t="s">
         <v>39</v>
@@ -1724,7 +1724,7 @@
         <v>39</v>
       </c>
       <c r="AG5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="AH5" t="s">
         <v>39</v>
@@ -1742,24 +1742,24 @@
         <v>39</v>
       </c>
       <c r="AM5" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
         <v>39</v>
@@ -1831,7 +1831,7 @@
         <v>39</v>
       </c>
       <c r="AC6" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="AD6" t="s">
         <v>39</v>
@@ -1843,7 +1843,7 @@
         <v>39</v>
       </c>
       <c r="AG6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="AH6" t="s">
         <v>39</v>
@@ -1861,24 +1861,24 @@
         <v>39</v>
       </c>
       <c r="AM6" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
         <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -1950,7 +1950,7 @@
         <v>39</v>
       </c>
       <c r="AC7" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="AD7" t="s">
         <v>39</v>
@@ -1962,7 +1962,7 @@
         <v>39</v>
       </c>
       <c r="AG7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="AH7" t="s">
         <v>39</v>
@@ -1980,24 +1980,24 @@
         <v>39</v>
       </c>
       <c r="AM7" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
         <v>39</v>
@@ -2069,7 +2069,7 @@
         <v>39</v>
       </c>
       <c r="AC8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="AD8" t="s">
         <v>39</v>
@@ -2081,7 +2081,7 @@
         <v>39</v>
       </c>
       <c r="AG8" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="AH8" t="s">
         <v>39</v>
@@ -2099,24 +2099,24 @@
         <v>39</v>
       </c>
       <c r="AM8" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
         <v>39</v>
@@ -2188,19 +2188,19 @@
         <v>39</v>
       </c>
       <c r="AC9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AD9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AE9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AF9" t="s">
         <v>39</v>
       </c>
       <c r="AG9" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="AH9" t="s">
         <v>39</v>
@@ -2218,7 +2218,7 @@
         <v>39</v>
       </c>
       <c r="AM9" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>